<commit_message>
Aulas do primeiro módulo - multiplas-planilhas - finalizando o módulo
</commit_message>
<xml_diff>
--- a/aula-multiplas-planilhas.xlsx
+++ b/aula-multiplas-planilhas.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Troca de arquivos\Curso_Excel\02 Primeiros passos sobre planilha eletrônica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10125" windowHeight="6780" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pedido 9120" sheetId="2" r:id="rId1"/>
     <sheet name="Pedido 8340" sheetId="5" r:id="rId2"/>
-    <sheet name="Resumo" sheetId="7" r:id="rId3"/>
+    <sheet name="Pedido 7635" sheetId="8" r:id="rId3"/>
+    <sheet name="Resumo" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Pedido número 9120</t>
   </si>
@@ -74,6 +75,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pedido número 7635</t>
+  </si>
+  <si>
+    <t>Acessar valores de outras tabelas: insere o sinal = clica em cima da tabela desejada clica no item que deseja que apareça na outra tabela e aberta o enter.</t>
   </si>
 </sst>
 </file>
@@ -81,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -148,11 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,9 +463,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -575,9 +588,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -674,9 +692,123 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <f>C4*D4-C4*D4*E4</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5" si="0">C5*D5-C5*D5*E5</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="3">
+        <f>F4+F5</f>
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="B2:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -685,17 +817,17 @@
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -703,7 +835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>9120</v>
       </c>
@@ -712,7 +844,7 @@
         <v>949.97500000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>8340</v>
       </c>
@@ -721,18 +853,38 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>7635</v>
+      </c>
+      <c r="C7" s="3">
+        <f>'Pedido 7635'!F7</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3">
-        <f>C5+C6</f>
-        <v>1121.9749999999999</v>
-      </c>
+      <c r="C9" s="3">
+        <f>C5+C6+C7</f>
+        <v>1401.9749999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B12:G12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>